<commit_message>
added input check from user + updated excel test cases
</commit_message>
<xml_diff>
--- a/doc/Test cases.xlsx
+++ b/doc/Test cases.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\virgi\Snack-Automat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\virgi\Snack-Automat\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5AE246-D511-4CB9-97BC-E3FC563007C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62C203E-7C3F-493A-9EF6-58ADEF312D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11580" xr2:uid="{5B3F2C69-5835-4169-A03A-AFBC5E7BAFD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
   <si>
     <t>Nr.</t>
   </si>
@@ -117,13 +118,109 @@
   </si>
   <si>
     <t>You can buy the product again</t>
+  </si>
+  <si>
+    <t>Return change</t>
+  </si>
+  <si>
+    <t>A user can insert more money then needed</t>
+  </si>
+  <si>
+    <t>The change will be returned to the user</t>
+  </si>
+  <si>
+    <t>Give money back</t>
+  </si>
+  <si>
+    <t>Anytime the user can cancel the process and get the money back</t>
+  </si>
+  <si>
+    <t>When the user press quit, he can get the money back</t>
+  </si>
+  <si>
+    <t>Noser Young</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Nr. 1</t>
+  </si>
+  <si>
+    <t>No blank lines</t>
+  </si>
+  <si>
+    <t>Nr. 2</t>
+  </si>
+  <si>
+    <t>No comments</t>
+  </si>
+  <si>
+    <t>Nr. 3</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Correct access modifiers</t>
+  </si>
+  <si>
+    <t>Nr. 4</t>
+  </si>
+  <si>
+    <t>Correct casing</t>
+  </si>
+  <si>
+    <t>Nr. 5</t>
+  </si>
+  <si>
+    <t>There are not more blank lines than needed</t>
+  </si>
+  <si>
+    <t>Only important commets in the code</t>
+  </si>
+  <si>
+    <t>The access modifers are right chosen</t>
+  </si>
+  <si>
+    <t>Correct casing is used for name of a class, method</t>
+  </si>
+  <si>
+    <t>Test case number</t>
+  </si>
+  <si>
+    <t>Test case designation</t>
+  </si>
+  <si>
+    <t>Request number</t>
+  </si>
+  <si>
+    <t>Test environment</t>
+  </si>
+  <si>
+    <t>Steps:</t>
+  </si>
+  <si>
+    <t>Clean code test</t>
+  </si>
+  <si>
+    <t>Date of the test execution</t>
+  </si>
+  <si>
+    <t>Timofey, Tsering, Virginia</t>
+  </si>
+  <si>
+    <t>Functional test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,8 +228,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,8 +256,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -154,13 +271,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -179,8 +364,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B790EC74-5E6F-4E8D-9915-089C291A84A5}" name="Table1" displayName="Table1" ref="A1:F8" totalsRowShown="0">
-  <autoFilter ref="A1:F8" xr:uid="{B790EC74-5E6F-4E8D-9915-089C291A84A5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B790EC74-5E6F-4E8D-9915-089C291A84A5}" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0">
+  <autoFilter ref="A1:F11" xr:uid="{B790EC74-5E6F-4E8D-9915-089C291A84A5}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9DF7DB54-CB25-46E7-8E38-A63EFE3A7BBB}" name="Nr."/>
     <tableColumn id="2" xr3:uid="{0516A2A8-E6B5-403D-9BCE-44B8B45C1867}" name="Test"/>
@@ -188,6 +373,29 @@
     <tableColumn id="4" xr3:uid="{A7902A93-D285-436D-9F61-85D428B305A9}" name="Expected Output"/>
     <tableColumn id="5" xr3:uid="{FA1E0663-0516-4CB7-AE18-CED843C3FF58}" name="Result obtained"/>
     <tableColumn id="6" xr3:uid="{EFFB6D62-CBF1-4CAF-9513-D7B10BCC476F}" name="Status"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{52147BB9-115F-46F5-9738-CBF6009F051E}" name="Table5" displayName="Table5" ref="B16:D21" totalsRowShown="0">
+  <autoFilter ref="B16:D21" xr:uid="{52147BB9-115F-46F5-9738-CBF6009F051E}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{398D7912-DCF9-46D4-83D4-2E833458D7C0}" name="Nr."/>
+    <tableColumn id="2" xr3:uid="{8725375B-3646-423B-A44A-044A8665ACB1}" name="Test"/>
+    <tableColumn id="3" xr3:uid="{194BDE1C-781A-46B2-8119-BFEB59FD6D84}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FB0E11E9-3BDF-4676-8909-7A30CF23F832}" name="Table6" displayName="Table6" ref="G16:H22" totalsRowShown="0">
+  <autoFilter ref="G16:H22" xr:uid="{FB0E11E9-3BDF-4676-8909-7A30CF23F832}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{FEF1B0C8-0833-4A4D-ADED-2540D45F62FF}" name="Test case number"/>
+    <tableColumn id="2" xr3:uid="{E90A92A1-45FF-4394-AFF7-F3601F87A0BB}" name="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -490,22 +698,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55D57CB-3B8F-4677-8319-0CD9B51F9AE4}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="2" max="2" width="25.2265625" customWidth="1"/>
-    <col min="3" max="3" width="51.7265625" customWidth="1"/>
-    <col min="4" max="4" width="47.953125" customWidth="1"/>
+    <col min="3" max="3" width="54.6328125" customWidth="1"/>
+    <col min="4" max="4" width="55.453125" customWidth="1"/>
     <col min="5" max="5" width="30.08984375" customWidth="1"/>
     <col min="6" max="6" width="14.453125" customWidth="1"/>
+    <col min="12" max="12" width="28.6796875" customWidth="1"/>
+    <col min="13" max="13" width="26.54296875" customWidth="1"/>
+    <col min="15" max="15" width="27.26953125" customWidth="1"/>
+    <col min="16" max="16" width="31.1328125" customWidth="1"/>
+    <col min="17" max="17" width="27.40625" customWidth="1"/>
+    <col min="18" max="18" width="30.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -525,7 +739,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="22.75" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:16" ht="22.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -538,8 +752,14 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="22.75" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="O2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="22.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -552,8 +772,14 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="O3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -566,8 +792,14 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="22.75" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="O4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="P4" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="22.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -580,8 +812,14 @@
       <c r="D5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="O5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -594,8 +832,14 @@
       <c r="D6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="O6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="P6" s="11">
+        <v>44910</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -608,8 +852,14 @@
       <c r="D7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="O7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -622,11 +872,179 @@
       <c r="D8" t="s">
         <v>26</v>
       </c>
+      <c r="O8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="P8" s="4"/>
+    </row>
+    <row r="9" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712CEDD2-5549-42AE-990E-21C2CA5AF94A}">
+  <dimension ref="B16:H22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="2" max="2" width="9.76953125" customWidth="1"/>
+    <col min="3" max="3" width="24.36328125" customWidth="1"/>
+    <col min="4" max="4" width="46.36328125" customWidth="1"/>
+    <col min="5" max="5" width="45.54296875" customWidth="1"/>
+    <col min="7" max="7" width="39.86328125" customWidth="1"/>
+    <col min="8" max="8" width="24.7265625" customWidth="1"/>
+    <col min="9" max="9" width="19.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="16" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="22.75" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="8">
+        <v>44910</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="G22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed every error output to normal output
</commit_message>
<xml_diff>
--- a/doc/Test cases.xlsx
+++ b/doc/Test cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\virgi\Snack-Automat\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Snack-Automat\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62C203E-7C3F-493A-9EF6-58ADEF312D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048E7877-52FB-41EA-942F-2696E2724DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11580" xr2:uid="{5B3F2C69-5835-4169-A03A-AFBC5E7BAFD8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{5B3F2C69-5835-4169-A03A-AFBC5E7BAFD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
   <si>
     <t>Nr.</t>
   </si>
@@ -93,15 +93,9 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Exchange a product</t>
-  </si>
-  <si>
     <t>Change a products price</t>
   </si>
   <si>
-    <t>Exchange an existing product for another one (+ secret key)</t>
-  </si>
-  <si>
     <t>Change a products price (+secret key)</t>
   </si>
   <si>
@@ -214,6 +208,39 @@
   </si>
   <si>
     <t>Functional test</t>
+  </si>
+  <si>
+    <t>Replace a product</t>
+  </si>
+  <si>
+    <t>Replace an existing product for another one (+ secret key)</t>
+  </si>
+  <si>
+    <t>decrease amount of Item</t>
+  </si>
+  <si>
+    <t>decrease an amount of the chosen Item in the Vending Machine</t>
+  </si>
+  <si>
+    <t>The Amount will decrease from the Vending machine</t>
+  </si>
+  <si>
+    <t>Stop the User from buying</t>
+  </si>
+  <si>
+    <t>If the Vending Machine is Empty, the User won't able to so anything</t>
+  </si>
+  <si>
+    <t>At the buying Process, if empty, won't able to do anything</t>
+  </si>
+  <si>
+    <t>able to quit buying any Time</t>
+  </si>
+  <si>
+    <t>The User shoulb be able to quit in the Process Stage</t>
+  </si>
+  <si>
+    <t>inputing -1 should stop the process and return the Money</t>
   </si>
 </sst>
 </file>
@@ -327,10 +354,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -340,10 +367,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -364,8 +391,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B790EC74-5E6F-4E8D-9915-089C291A84A5}" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0">
-  <autoFilter ref="A1:F11" xr:uid="{B790EC74-5E6F-4E8D-9915-089C291A84A5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B790EC74-5E6F-4E8D-9915-089C291A84A5}" name="Table1" displayName="Table1" ref="A1:F14" totalsRowShown="0">
+  <autoFilter ref="A1:F14" xr:uid="{B790EC74-5E6F-4E8D-9915-089C291A84A5}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9DF7DB54-CB25-46E7-8E38-A63EFE3A7BBB}" name="Nr."/>
     <tableColumn id="2" xr3:uid="{0516A2A8-E6B5-403D-9BCE-44B8B45C1867}" name="Test"/>
@@ -698,28 +725,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55D57CB-3B8F-4677-8319-0CD9B51F9AE4}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.2265625" customWidth="1"/>
-    <col min="3" max="3" width="54.6328125" customWidth="1"/>
-    <col min="4" max="4" width="55.453125" customWidth="1"/>
-    <col min="5" max="5" width="30.08984375" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
-    <col min="12" max="12" width="28.6796875" customWidth="1"/>
-    <col min="13" max="13" width="26.54296875" customWidth="1"/>
-    <col min="15" max="15" width="27.26953125" customWidth="1"/>
-    <col min="16" max="16" width="31.1328125" customWidth="1"/>
-    <col min="17" max="17" width="27.40625" customWidth="1"/>
-    <col min="18" max="18" width="30.36328125" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="60.85546875" customWidth="1"/>
+    <col min="4" max="4" width="55.42578125" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="28.7109375" customWidth="1"/>
+    <col min="13" max="13" width="26.5703125" customWidth="1"/>
+    <col min="15" max="15" width="27.28515625" customWidth="1"/>
+    <col min="16" max="16" width="31.140625" customWidth="1"/>
+    <col min="17" max="17" width="27.42578125" customWidth="1"/>
+    <col min="18" max="18" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -739,7 +766,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="22.75" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:16" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -753,13 +780,13 @@
         <v>7</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="22.75" customHeight="1" x14ac:dyDescent="0.75">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -773,13 +800,13 @@
         <v>10</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -793,13 +820,13 @@
         <v>13</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P4" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="22.75" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:16" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -813,101 +840,143 @@
         <v>16</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
       <c r="O6" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="P6" s="11">
         <v>44910</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
       <c r="O7" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
       <c r="O8" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+    </row>
+    <row r="10" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
       <c r="D10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -927,18 +996,18 @@
       <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.76953125" customWidth="1"/>
-    <col min="3" max="3" width="24.36328125" customWidth="1"/>
-    <col min="4" max="4" width="46.36328125" customWidth="1"/>
-    <col min="5" max="5" width="45.54296875" customWidth="1"/>
-    <col min="7" max="7" width="39.86328125" customWidth="1"/>
-    <col min="8" max="8" width="24.7265625" customWidth="1"/>
-    <col min="9" max="9" width="19.1796875" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="46.42578125" customWidth="1"/>
+    <col min="5" max="5" width="45.5703125" customWidth="1"/>
+    <col min="7" max="7" width="39.85546875" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="16" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="16" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>0</v>
       </c>
@@ -946,97 +1015,97 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" t="s">
         <v>50</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17" t="s">
-        <v>51</v>
-      </c>
-      <c r="H17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="22.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G18" t="s">
-        <v>52</v>
       </c>
       <c r="H18" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="19" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
         <v>40</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
         <v>42</v>
       </c>
-      <c r="D19" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" t="s">
-        <v>44</v>
-      </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H20" s="8">
         <v>44910</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="21" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update excel functional test + cleaned code
</commit_message>
<xml_diff>
--- a/doc/Test cases.xlsx
+++ b/doc/Test cases.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Snack-Automat\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\virgi\Snack-Automat\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048E7877-52FB-41EA-942F-2696E2724DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E78D80-6BA1-4C4B-BBE5-FBC625AB8DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{5B3F2C69-5835-4169-A03A-AFBC5E7BAFD8}"/>
+    <workbookView minimized="1" xWindow="34560" yWindow="-15690" windowWidth="4800" windowHeight="2760" activeTab="1" xr2:uid="{5B3F2C69-5835-4169-A03A-AFBC5E7BAFD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="81">
   <si>
     <t>Nr.</t>
   </si>
@@ -69,9 +70,6 @@
     <t>Enter secret key and fill up the machine</t>
   </si>
   <si>
-    <t>The machine has a x number of each product in it</t>
-  </si>
-  <si>
     <t>Buy a product</t>
   </si>
   <si>
@@ -96,9 +94,6 @@
     <t>Change a products price</t>
   </si>
   <si>
-    <t>Change a products price (+secret key)</t>
-  </si>
-  <si>
     <t>New product is visible on the screen</t>
   </si>
   <si>
@@ -108,9 +103,6 @@
     <t>Refill vending machine</t>
   </si>
   <si>
-    <t>Refill machine in case a product isn't on stack</t>
-  </si>
-  <si>
     <t>You can buy the product again</t>
   </si>
   <si>
@@ -123,15 +115,6 @@
     <t>The change will be returned to the user</t>
   </si>
   <si>
-    <t>Give money back</t>
-  </si>
-  <si>
-    <t>Anytime the user can cancel the process and get the money back</t>
-  </si>
-  <si>
-    <t>When the user press quit, he can get the money back</t>
-  </si>
-  <si>
     <t>Noser Young</t>
   </si>
   <si>
@@ -213,34 +196,91 @@
     <t>Replace a product</t>
   </si>
   <si>
-    <t>Replace an existing product for another one (+ secret key)</t>
-  </si>
-  <si>
-    <t>decrease amount of Item</t>
-  </si>
-  <si>
-    <t>decrease an amount of the chosen Item in the Vending Machine</t>
-  </si>
-  <si>
     <t>The Amount will decrease from the Vending machine</t>
   </si>
   <si>
     <t>Stop the User from buying</t>
   </si>
   <si>
-    <t>If the Vending Machine is Empty, the User won't able to so anything</t>
-  </si>
-  <si>
-    <t>At the buying Process, if empty, won't able to do anything</t>
-  </si>
-  <si>
-    <t>able to quit buying any Time</t>
-  </si>
-  <si>
-    <t>The User shoulb be able to quit in the Process Stage</t>
-  </si>
-  <si>
-    <t>inputing -1 should stop the process and return the Money</t>
+    <t>Decrease amount of Item</t>
+  </si>
+  <si>
+    <t>Decrease an amount of the chosen Item in the Vending Machine</t>
+  </si>
+  <si>
+    <t>If the Vending Machine is empty the user won't able to so anything</t>
+  </si>
+  <si>
+    <t>At the buying process, if empty, won't be able to do anything</t>
+  </si>
+  <si>
+    <t>Able to quit buying any time</t>
+  </si>
+  <si>
+    <t>Inputing -1 should stop the process and return the Money</t>
+  </si>
+  <si>
+    <t>The user should be able to quit anytime during the process stage</t>
+  </si>
+  <si>
+    <t>The user enters the admin mode and is able to modify things</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>The machine is empty at first, the user can fill it up</t>
+  </si>
+  <si>
+    <t>Admin can add as many items as wanted</t>
+  </si>
+  <si>
+    <t>In process</t>
+  </si>
+  <si>
+    <t>You get the item after inserting the money</t>
+  </si>
+  <si>
+    <t>User experience was not satisfied</t>
+  </si>
+  <si>
+    <t>Replace an existing product for another one (admin)</t>
+  </si>
+  <si>
+    <t>Change a products price (admin)</t>
+  </si>
+  <si>
+    <t>Refill machine in case a product isn't on stack (admin)</t>
+  </si>
+  <si>
+    <t>Product + name, amount, price can be changed</t>
+  </si>
+  <si>
+    <t>Just the price of an item alone can also be changed</t>
+  </si>
+  <si>
+    <t>Admin chan refill an item but it doesn't show the changes</t>
+  </si>
+  <si>
+    <t>Easy to quit buying by entering -1</t>
+  </si>
+  <si>
+    <t>The money is returned to the user but not shown on screen</t>
+  </si>
+  <si>
+    <t>Not working</t>
+  </si>
+  <si>
+    <t>At the beginning is machine empty, user not able to buy</t>
+  </si>
+  <si>
+    <t>Correct grammar</t>
+  </si>
+  <si>
+    <t>Words are written right</t>
+  </si>
+  <si>
+    <t>..</t>
   </si>
 </sst>
 </file>
@@ -391,8 +431,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B790EC74-5E6F-4E8D-9915-089C291A84A5}" name="Table1" displayName="Table1" ref="A1:F14" totalsRowShown="0">
-  <autoFilter ref="A1:F14" xr:uid="{B790EC74-5E6F-4E8D-9915-089C291A84A5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B790EC74-5E6F-4E8D-9915-089C291A84A5}" name="Table1" displayName="Table1" ref="A1:F12" totalsRowShown="0">
+  <autoFilter ref="A1:F12" xr:uid="{B790EC74-5E6F-4E8D-9915-089C291A84A5}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9DF7DB54-CB25-46E7-8E38-A63EFE3A7BBB}" name="Nr."/>
     <tableColumn id="2" xr3:uid="{0516A2A8-E6B5-403D-9BCE-44B8B45C1867}" name="Test"/>
@@ -406,20 +453,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{52147BB9-115F-46F5-9738-CBF6009F051E}" name="Table5" displayName="Table5" ref="B16:D21" totalsRowShown="0">
-  <autoFilter ref="B16:D21" xr:uid="{52147BB9-115F-46F5-9738-CBF6009F051E}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{52147BB9-115F-46F5-9738-CBF6009F051E}" name="Table5" displayName="Table5" ref="B16:E21" totalsRowShown="0">
+  <autoFilter ref="B16:E21" xr:uid="{52147BB9-115F-46F5-9738-CBF6009F051E}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{398D7912-DCF9-46D4-83D4-2E833458D7C0}" name="Nr."/>
     <tableColumn id="2" xr3:uid="{8725375B-3646-423B-A44A-044A8665ACB1}" name="Test"/>
-    <tableColumn id="3" xr3:uid="{194BDE1C-781A-46B2-8119-BFEB59FD6D84}" name="Description"/>
+    <tableColumn id="4" xr3:uid="{5E59AB23-1073-42E0-9269-14F5DE2BEEBE}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{194BDE1C-781A-46B2-8119-BFEB59FD6D84}" name=".."/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FB0E11E9-3BDF-4676-8909-7A30CF23F832}" name="Table6" displayName="Table6" ref="G16:H22" totalsRowShown="0">
-  <autoFilter ref="G16:H22" xr:uid="{FB0E11E9-3BDF-4676-8909-7A30CF23F832}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FB0E11E9-3BDF-4676-8909-7A30CF23F832}" name="Table6" displayName="Table6" ref="I16:J22" totalsRowShown="0">
+  <autoFilter ref="I16:J22" xr:uid="{FB0E11E9-3BDF-4676-8909-7A30CF23F832}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{FEF1B0C8-0833-4A4D-ADED-2540D45F62FF}" name="Test case number"/>
     <tableColumn id="2" xr3:uid="{E90A92A1-45FF-4394-AFF7-F3601F87A0BB}" name="1"/>
@@ -725,28 +773,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55D57CB-3B8F-4677-8319-0CD9B51F9AE4}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="60.85546875" customWidth="1"/>
-    <col min="4" max="4" width="55.42578125" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="12" max="12" width="28.7109375" customWidth="1"/>
-    <col min="13" max="13" width="26.5703125" customWidth="1"/>
-    <col min="15" max="15" width="27.28515625" customWidth="1"/>
-    <col min="16" max="16" width="31.140625" customWidth="1"/>
-    <col min="17" max="17" width="27.42578125" customWidth="1"/>
-    <col min="18" max="18" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" customWidth="1"/>
+    <col min="3" max="3" width="60.86328125" customWidth="1"/>
+    <col min="4" max="4" width="55.40625" customWidth="1"/>
+    <col min="5" max="5" width="50.7265625" customWidth="1"/>
+    <col min="6" max="6" width="14.40625" customWidth="1"/>
+    <col min="12" max="12" width="28.7265625" customWidth="1"/>
+    <col min="13" max="13" width="26.54296875" customWidth="1"/>
+    <col min="15" max="15" width="27.26953125" customWidth="1"/>
+    <col min="16" max="16" width="31.1328125" customWidth="1"/>
+    <col min="17" max="17" width="27.40625" customWidth="1"/>
+    <col min="18" max="18" width="30.40625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -763,10 +811,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="22.7" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -779,14 +827,20 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
       <c r="O2" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="22.7" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -797,188 +851,230 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" t="s">
+        <v>62</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="P4" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="22.7" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
-        <v>16</v>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" t="s">
+        <v>65</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" t="s">
+        <v>62</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="P6" s="11">
         <v>44910</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
-        <v>21</v>
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" t="s">
+        <v>65</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="E11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" t="s">
         <v>62</v>
       </c>
-      <c r="C12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-    </row>
+    </row>
+    <row r="13" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.75"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -990,24 +1086,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712CEDD2-5549-42AE-990E-21C2CA5AF94A}">
-  <dimension ref="B16:H22"/>
+  <dimension ref="B16:J22"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="136" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
-    <col min="4" max="4" width="46.42578125" customWidth="1"/>
-    <col min="5" max="5" width="45.5703125" customWidth="1"/>
-    <col min="7" max="7" width="39.85546875" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" customWidth="1"/>
+    <col min="3" max="3" width="24.40625" customWidth="1"/>
+    <col min="4" max="4" width="47.08984375" customWidth="1"/>
+    <col min="5" max="6" width="46.40625" customWidth="1"/>
+    <col min="7" max="7" width="45.54296875" customWidth="1"/>
+    <col min="9" max="9" width="39.86328125" customWidth="1"/>
+    <col min="10" max="10" width="24.7265625" customWidth="1"/>
+    <col min="11" max="11" width="19.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="16" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B16" t="s">
         <v>0</v>
       </c>
@@ -1015,97 +1112,106 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" t="s">
+        <v>80</v>
+      </c>
+      <c r="I16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="22.7" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
         <v>39</v>
       </c>
-      <c r="G16" t="s">
+      <c r="I18" t="s">
+        <v>44</v>
+      </c>
+      <c r="J18" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="J20" s="8">
+        <v>44910</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" t="s">
+        <v>79</v>
+      </c>
+      <c r="I21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" t="s">
         <v>49</v>
       </c>
-      <c r="H17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" t="s">
-        <v>50</v>
-      </c>
-      <c r="H18" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" t="s">
+    </row>
+    <row r="22" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="I22" t="s">
         <v>46</v>
-      </c>
-      <c r="G19" t="s">
-        <v>51</v>
-      </c>
-      <c r="H19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" t="s">
-        <v>54</v>
-      </c>
-      <c r="H20" s="8">
-        <v>44910</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>43</v>
-      </c>
-      <c r="G21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G22" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel test cases test 2 finished
</commit_message>
<xml_diff>
--- a/doc/Test cases.xlsx
+++ b/doc/Test cases.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\virgi\Snack-Automat\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E78D80-6BA1-4C4B-BBE5-FBC625AB8DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EE39AC-2882-4647-A20B-1896826DF282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="34560" yWindow="-15690" windowWidth="4800" windowHeight="2760" activeTab="1" xr2:uid="{5B3F2C69-5835-4169-A03A-AFBC5E7BAFD8}"/>
+    <workbookView xWindow="28770" yWindow="-18120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{5B3F2C69-5835-4169-A03A-AFBC5E7BAFD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="81">
   <si>
     <t>Nr.</t>
   </si>
@@ -280,7 +279,7 @@
     <t>Words are written right</t>
   </si>
   <si>
-    <t>..</t>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -454,12 +453,17 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{52147BB9-115F-46F5-9738-CBF6009F051E}" name="Table5" displayName="Table5" ref="B16:E21" totalsRowShown="0">
-  <autoFilter ref="B16:E21" xr:uid="{52147BB9-115F-46F5-9738-CBF6009F051E}"/>
+  <autoFilter ref="B16:E21" xr:uid="{52147BB9-115F-46F5-9738-CBF6009F051E}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{398D7912-DCF9-46D4-83D4-2E833458D7C0}" name="Nr."/>
     <tableColumn id="2" xr3:uid="{8725375B-3646-423B-A44A-044A8665ACB1}" name="Test"/>
     <tableColumn id="4" xr3:uid="{5E59AB23-1073-42E0-9269-14F5DE2BEEBE}" name="Description"/>
-    <tableColumn id="3" xr3:uid="{194BDE1C-781A-46B2-8119-BFEB59FD6D84}" name=".."/>
+    <tableColumn id="3" xr3:uid="{194BDE1C-781A-46B2-8119-BFEB59FD6D84}" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -467,10 +471,13 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FB0E11E9-3BDF-4676-8909-7A30CF23F832}" name="Table6" displayName="Table6" ref="I16:J22" totalsRowShown="0">
-  <autoFilter ref="I16:J22" xr:uid="{FB0E11E9-3BDF-4676-8909-7A30CF23F832}"/>
+  <autoFilter ref="I16:J22" xr:uid="{FB0E11E9-3BDF-4676-8909-7A30CF23F832}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{FEF1B0C8-0833-4A4D-ADED-2540D45F62FF}" name="Test case number"/>
-    <tableColumn id="2" xr3:uid="{E90A92A1-45FF-4394-AFF7-F3601F87A0BB}" name="1"/>
+    <tableColumn id="2" xr3:uid="{E90A92A1-45FF-4394-AFF7-F3601F87A0BB}" name="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1088,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712CEDD2-5549-42AE-990E-21C2CA5AF94A}">
   <dimension ref="B16:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="136" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="136" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1097,7 +1104,8 @@
     <col min="2" max="2" width="9.7265625" customWidth="1"/>
     <col min="3" max="3" width="24.40625" customWidth="1"/>
     <col min="4" max="4" width="47.08984375" customWidth="1"/>
-    <col min="5" max="6" width="46.40625" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" customWidth="1"/>
+    <col min="6" max="6" width="46.40625" customWidth="1"/>
     <col min="7" max="7" width="45.54296875" customWidth="1"/>
     <col min="9" max="9" width="39.86328125" customWidth="1"/>
     <col min="10" max="10" width="24.7265625" customWidth="1"/>
@@ -1115,13 +1123,13 @@
         <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="I16" t="s">
         <v>42</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
@@ -1134,6 +1142,9 @@
       <c r="D17" t="s">
         <v>38</v>
       </c>
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
       <c r="I17" t="s">
         <v>43</v>
       </c>
@@ -1151,6 +1162,9 @@
       <c r="D18" t="s">
         <v>39</v>
       </c>
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
       <c r="I18" t="s">
         <v>44</v>
       </c>
@@ -1168,6 +1182,9 @@
       <c r="D19" t="s">
         <v>40</v>
       </c>
+      <c r="E19" t="s">
+        <v>62</v>
+      </c>
       <c r="I19" t="s">
         <v>45</v>
       </c>
@@ -1185,6 +1202,9 @@
       <c r="D20" t="s">
         <v>41</v>
       </c>
+      <c r="E20" t="s">
+        <v>62</v>
+      </c>
       <c r="I20" t="s">
         <v>48</v>
       </c>
@@ -1201,6 +1221,9 @@
       </c>
       <c r="D21" t="s">
         <v>79</v>
+      </c>
+      <c r="E21" t="s">
+        <v>62</v>
       </c>
       <c r="I21" t="s">
         <v>26</v>

</xml_diff>